<commit_message>
retinker and add LR estimation
</commit_message>
<xml_diff>
--- a/Assessments/answers_Intermtn MS4 1 Transcript.xlsx
+++ b/Assessments/answers_Intermtn MS4 1 Transcript.xlsx
@@ -450,20 +450,20 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="b">
-        <v>0</v>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Do you have any PMHx? (counts as 2 independent minor features)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Pain not worse with exertion (requires they clarify exercise 1hr after meal)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Do you have any PMHx? (counts as 2 independent minor features)</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,9 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>no associated shortness of breath</t>
@@ -485,7 +487,7 @@
     </row>
     <row r="6">
       <c r="A6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -517,12 +519,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Alternative cause of esoph dysphagia becomes obvious (food gets stuck or relieved by regurgitation of food)</t>
+          <t>Alternative cause of esoph dysphagia becomes obvious(food gets stuck or relieved by regurgitation of food)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="b">
+        <v>1</v>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>no prior CAD</t>
@@ -546,7 +550,9 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>no prior MI</t>
@@ -717,9 +723,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="b">
-        <v>1</v>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
           <t>Alternative cause becomes obvious: esoph dysphagia (food gets stuck or relieved by regurgitation of food)</t>
@@ -753,9 +757,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="b">
-        <v>1</v>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
           <t>No dry cough</t>
@@ -810,7 +812,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Food gets stuck</t>
@@ -1062,7 +1066,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Difficulty swallowing liquids</t>
@@ -1086,7 +1092,9 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="b">
+        <v>1</v>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>no associated shortness of breath</t>

</xml_diff>